<commit_message>
unit and every year
</commit_message>
<xml_diff>
--- a/meta_stra_framwork/result/single/single.xlsx
+++ b/meta_stra_framwork/result/single/single.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>strategy_name</t>
   </si>
@@ -88,10 +88,94 @@
     <t>stock_num</t>
   </si>
   <si>
-    <t>['close_EMA_7#close_EMA_15#1&amp;diff*close_EMA_15#close_EMA_25#1&amp;diff*close_EMA_15#2#1&amp;trend*close_EMA_25#2#1&amp;trend*MACD#0#1&amp;thre*close#close_shift_4#1&amp;diff*K#40#1&amp;thre&amp;HS', 'MACD#0#0&amp;thre+K#40#0&amp;thre&amp;HS']</t>
-  </si>
-  <si>
-    <t>['close_MA_5#close_MA_30#1&amp;cross', 'close_MA_5#1#0&amp;trend']</t>
+    <t>2016max_draw_down</t>
+  </si>
+  <si>
+    <t>2016Sharpe</t>
+  </si>
+  <si>
+    <t>2016Total_Return</t>
+  </si>
+  <si>
+    <t>2017max_draw_down</t>
+  </si>
+  <si>
+    <t>2017Sharpe</t>
+  </si>
+  <si>
+    <t>2017Total_Return</t>
+  </si>
+  <si>
+    <t>2018max_draw_down</t>
+  </si>
+  <si>
+    <t>2018Sharpe</t>
+  </si>
+  <si>
+    <t>2018Total_Return</t>
+  </si>
+  <si>
+    <t>2019max_draw_down</t>
+  </si>
+  <si>
+    <t>2019Sharpe</t>
+  </si>
+  <si>
+    <t>2019Total_Return</t>
+  </si>
+  <si>
+    <t>2010max_draw_down</t>
+  </si>
+  <si>
+    <t>2010Sharpe</t>
+  </si>
+  <si>
+    <t>2010Total_Return</t>
+  </si>
+  <si>
+    <t>2011max_draw_down</t>
+  </si>
+  <si>
+    <t>2011Sharpe</t>
+  </si>
+  <si>
+    <t>2011Total_Return</t>
+  </si>
+  <si>
+    <t>2012max_draw_down</t>
+  </si>
+  <si>
+    <t>2012Sharpe</t>
+  </si>
+  <si>
+    <t>2012Total_Return</t>
+  </si>
+  <si>
+    <t>2013max_draw_down</t>
+  </si>
+  <si>
+    <t>2013Sharpe</t>
+  </si>
+  <si>
+    <t>2013Total_Return</t>
+  </si>
+  <si>
+    <t>2014max_draw_down</t>
+  </si>
+  <si>
+    <t>2014Sharpe</t>
+  </si>
+  <si>
+    <t>2014Total_Return</t>
+  </si>
+  <si>
+    <t>2015max_draw_down</t>
+  </si>
+  <si>
+    <t>2015Sharpe</t>
+  </si>
+  <si>
+    <t>2015Total_Return</t>
   </si>
   <si>
     <t>['close#2#0&amp;trend&amp;HS*MACD#2#1&amp;trend*MB#2#1&amp;trend', 'close#2#1&amp;trend&amp;HS*MACD#2#0&amp;trend*MB#2#0&amp;trend']</t>
@@ -464,13 +548,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:BC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:55">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,70 +627,160 @@
       <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:55">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="G2">
         <v>100000000</v>
       </c>
       <c r="H2">
-        <v>0.024</v>
+        <v>-0.047</v>
       </c>
       <c r="I2">
-        <v>0.131</v>
+        <v>0.213</v>
       </c>
       <c r="J2">
-        <v>0.265</v>
+        <v>-0.417</v>
       </c>
       <c r="K2">
-        <v>0.004</v>
+        <v>-0.332</v>
       </c>
       <c r="L2">
-        <v>0.152</v>
+        <v>0.14</v>
       </c>
       <c r="M2">
-        <v>0.228</v>
+        <v>0.204</v>
       </c>
       <c r="N2">
-        <v>0.005</v>
+        <v>-0.484</v>
       </c>
       <c r="O2">
-        <v>0.104</v>
+        <v>0.099</v>
       </c>
       <c r="P2">
-        <v>0.145</v>
+        <v>0.264</v>
       </c>
       <c r="Q2">
-        <v>158523666.303</v>
+        <v>88091211.057</v>
       </c>
       <c r="R2">
-        <v>158523666.303</v>
+        <v>49831259.057</v>
       </c>
       <c r="S2">
-        <v>0.585</v>
+        <v>-0.119</v>
       </c>
       <c r="T2">
-        <v>0.055</v>
+        <v>-0.015</v>
       </c>
       <c r="U2">
-        <v>1.585</v>
+        <v>0.881</v>
       </c>
       <c r="V2">
         <v>100000000</v>
@@ -620,159 +794,95 @@
       <c r="Y2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3">
-        <v>100000000</v>
-      </c>
-      <c r="H3">
-        <v>-0.034</v>
-      </c>
-      <c r="I3">
-        <v>0.001</v>
-      </c>
-      <c r="J3">
-        <v>-15.155</v>
-      </c>
-      <c r="K3">
-        <v>-0.259</v>
-      </c>
-      <c r="L3">
-        <v>0.163</v>
-      </c>
-      <c r="M3">
-        <v>0.236</v>
-      </c>
-      <c r="N3">
-        <v>-0.375</v>
-      </c>
-      <c r="O3">
-        <v>0.002</v>
-      </c>
-      <c r="P3">
-        <v>0.027</v>
-      </c>
-      <c r="Q3">
-        <v>97530705.72499999</v>
-      </c>
-      <c r="R3">
-        <v>94194847.72499999</v>
-      </c>
-      <c r="S3">
-        <v>-0.025</v>
-      </c>
-      <c r="T3">
-        <v>-0.003</v>
-      </c>
-      <c r="U3">
-        <v>0.975</v>
-      </c>
-      <c r="V3">
-        <v>100000000</v>
-      </c>
-      <c r="W3">
-        <v>0.296</v>
-      </c>
-      <c r="X3">
-        <v>0.031</v>
-      </c>
-      <c r="Y3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4">
-        <v>100000000</v>
-      </c>
-      <c r="H4">
-        <v>0.099</v>
-      </c>
-      <c r="I4">
-        <v>0.834</v>
-      </c>
-      <c r="J4">
-        <v>0.512</v>
-      </c>
-      <c r="K4">
-        <v>0.6909999999999999</v>
-      </c>
-      <c r="L4">
-        <v>0.094</v>
-      </c>
-      <c r="M4">
-        <v>0.137</v>
-      </c>
-      <c r="N4">
-        <v>1.003</v>
-      </c>
-      <c r="O4">
-        <v>0.236</v>
-      </c>
-      <c r="P4">
-        <v>0.431</v>
-      </c>
-      <c r="Q4">
-        <v>291370955.559</v>
-      </c>
-      <c r="R4">
-        <v>3937182.559</v>
-      </c>
-      <c r="S4">
-        <v>1.914</v>
-      </c>
-      <c r="T4">
-        <v>0.132</v>
-      </c>
-      <c r="U4">
-        <v>2.914</v>
-      </c>
-      <c r="V4">
-        <v>100000000</v>
-      </c>
-      <c r="W4">
-        <v>0.296</v>
-      </c>
-      <c r="X4">
-        <v>0.031</v>
-      </c>
-      <c r="Y4">
-        <v>300</v>
+      <c r="Z2">
+        <v>-0.02894975410990808</v>
+      </c>
+      <c r="AA2">
+        <v>-3.107489847887107</v>
+      </c>
+      <c r="AB2">
+        <v>-0.02709785221878536</v>
+      </c>
+      <c r="AC2">
+        <v>-0.0217394399126567</v>
+      </c>
+      <c r="AD2">
+        <v>-1.623911606464194</v>
+      </c>
+      <c r="AE2">
+        <v>-0.003202262032800722</v>
+      </c>
+      <c r="AF2">
+        <v>-0.05316637697251358</v>
+      </c>
+      <c r="AG2">
+        <v>-1.055135278043513</v>
+      </c>
+      <c r="AH2">
+        <v>-0.03170880461299627</v>
+      </c>
+      <c r="AI2">
+        <v>-0.02922422230346688</v>
+      </c>
+      <c r="AJ2">
+        <v>0.03502827710001312</v>
+      </c>
+      <c r="AK2">
+        <v>0.008826106126281938</v>
+      </c>
+      <c r="AL2">
+        <v>-0.006418789274236003</v>
+      </c>
+      <c r="AM2">
+        <v>-8.147546791460146</v>
+      </c>
+      <c r="AN2">
+        <v>-0.00567899999999999</v>
+      </c>
+      <c r="AO2">
+        <v>-0.07552901424177771</v>
+      </c>
+      <c r="AP2">
+        <v>-1.354468011130447</v>
+      </c>
+      <c r="AQ2">
+        <v>-0.04079165581336414</v>
+      </c>
+      <c r="AR2">
+        <v>-0.03247398836671433</v>
+      </c>
+      <c r="AS2">
+        <v>0.005330268371609658</v>
+      </c>
+      <c r="AT2">
+        <v>0.0315078934869428</v>
+      </c>
+      <c r="AU2">
+        <v>-0.2210335397267962</v>
+      </c>
+      <c r="AV2">
+        <v>-0.5630837943758764</v>
+      </c>
+      <c r="AW2">
+        <v>-0.08049721197145321</v>
+      </c>
+      <c r="AX2">
+        <v>-0.05298463322455915</v>
+      </c>
+      <c r="AY2">
+        <v>0.4750678959275052</v>
+      </c>
+      <c r="AZ2">
+        <v>0.08214970021503198</v>
+      </c>
+      <c r="BA2">
+        <v>-0.09566901722030163</v>
+      </c>
+      <c r="BB2">
+        <v>-0.4757281626791275</v>
+      </c>
+      <c r="BC2">
+        <v>-0.04926649772905754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>